<commit_message>
Updated to most recent data on all
</commit_message>
<xml_diff>
--- a/All Teraco Data/Operations DB1/Outputs/Data Analysis Results.xlsx
+++ b/All Teraco Data/Operations DB1/Outputs/Data Analysis Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="24">
   <si>
     <t>Total Incoming</t>
   </si>
@@ -483,7 +483,7 @@
         <v>44926</v>
       </c>
       <c r="B3">
-        <v>962865.8589999999</v>
+        <v>1332596.472</v>
       </c>
     </row>
   </sheetData>
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>957886</v>
+        <v>1311278</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -517,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>4979.858999999997</v>
+        <v>21318.47199999998</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>30.47493981194314</v>
+        <v>30.61730483104564</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -551,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>62.29297595232322</v>
+        <v>62.21831435255361</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -559,7 +559,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7.232084235733642</v>
+        <v>7.164380816400747</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +653,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3212,22 +3212,22 @@
         <v>190.078869047619</v>
       </c>
       <c r="E63">
-        <v>181.811394568756</v>
+        <v>185.2952572260893</v>
       </c>
       <c r="F63">
-        <v>8.267474478863022</v>
+        <v>4.783611821529718</v>
       </c>
       <c r="G63">
-        <v>28.07432099838474</v>
+        <v>24.59045834105143</v>
       </c>
       <c r="H63">
-        <v>1.045472807127809</v>
+        <v>1.025816158994793</v>
       </c>
       <c r="I63">
         <v>1.613921658484486</v>
       </c>
       <c r="J63">
-        <v>1.59242886934804</v>
+        <v>1.601485797877525</v>
       </c>
       <c r="K63">
         <v>384.6627083333275</v>
@@ -3250,171 +3250,171 @@
         <v>22</v>
       </c>
       <c r="D64">
-        <v>182.6049999999814</v>
+        <v>197.1086904762002</v>
       </c>
       <c r="E64">
-        <v>159.9790901560654</v>
+        <v>185.251300880667</v>
       </c>
       <c r="F64">
-        <v>22.62590984391593</v>
+        <v>11.85738959553322</v>
       </c>
       <c r="G64">
-        <v>50.70023084230067</v>
+        <v>36.44784793658465</v>
       </c>
       <c r="H64">
-        <v>1.14143041957448</v>
+        <v>1.064007051713884</v>
       </c>
       <c r="I64">
-        <v>1.575699045392223</v>
+        <v>1.625865329993205</v>
       </c>
       <c r="J64">
-        <v>1.516721999003159</v>
+        <v>1.595175665906781</v>
       </c>
       <c r="K64">
-        <v>383.6392500000075</v>
+        <v>386.3642678571466</v>
       </c>
       <c r="L64">
-        <v>604.5</v>
+        <v>628.1762678571429</v>
+      </c>
+      <c r="M64">
+        <v>43.3</v>
       </c>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="1">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="B65" s="3">
-        <v>44199</v>
+        <v>44640</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D65">
-        <v>134.2059718309705</v>
+        <v>193.7589999999895</v>
       </c>
       <c r="E65">
-        <v>154.6295022703841</v>
+        <v>177.3863615043983</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>16.37263849559127</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>52.82048643217593</v>
       </c>
       <c r="H65">
-        <v>0.8679195745990232</v>
+        <v>1.092299308451542</v>
       </c>
       <c r="I65">
-        <v>1.557589502491472</v>
+        <v>1.610143771924244</v>
       </c>
       <c r="J65">
-        <v>1.622575794915018</v>
+        <v>1.567829084876882</v>
       </c>
       <c r="K65">
-        <v>314.2744366197099</v>
+        <v>386.9256666666618</v>
       </c>
       <c r="L65">
-        <v>489.5105633802817</v>
+        <v>623.0059523809524</v>
       </c>
       <c r="M65">
-        <v>39.5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="1">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B66" s="3">
-        <v>44206</v>
+        <v>44647</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66">
-        <v>140.0087321428582</v>
+        <v>185.9311845238165</v>
       </c>
       <c r="E66">
-        <v>158.1917127966816</v>
+        <v>176.4547806342112</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>9.476403889605308</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>62.29689032178123</v>
       </c>
       <c r="H66">
-        <v>0.8850573122171492</v>
+        <v>1.053704432691171</v>
       </c>
       <c r="I66">
-        <v>1.572346885360321</v>
+        <v>1.588890099230065</v>
       </c>
       <c r="J66">
-        <v>1.62920241028032</v>
+        <v>1.564450753840787</v>
       </c>
       <c r="K66">
-        <v>319.8102678571428</v>
+        <v>387.7519523809564</v>
       </c>
       <c r="L66">
-        <v>502.8526785714286</v>
+        <v>616.0952380952381</v>
       </c>
       <c r="M66">
-        <v>41.4</v>
+        <v>29.1</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="1">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B67" s="3">
-        <v>44213</v>
+        <v>44654</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D67">
-        <v>144.4008035714284</v>
+        <v>199.28085416666</v>
       </c>
       <c r="E67">
-        <v>161.2506918173763</v>
+        <v>162.1769312969526</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>37.10392286970742</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>99.40081319148865</v>
       </c>
       <c r="H67">
-        <v>0.8955050173364142</v>
+        <v>1.228786687311086</v>
       </c>
       <c r="I67">
-        <v>1.495412542330898</v>
+        <v>1.630198047474724</v>
       </c>
       <c r="J67">
-        <v>1.548066889717883</v>
+        <v>1.53479309066739</v>
       </c>
       <c r="K67">
-        <v>320.0094404761912</v>
+        <v>388.9098020833238</v>
       </c>
       <c r="L67">
-        <v>478.546130952381</v>
-      </c>
-      <c r="M67">
-        <v>47.6</v>
+        <v>634</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B68" s="3">
-        <v>44220</v>
+        <v>44199</v>
       </c>
       <c r="C68" t="s">
         <v>23</v>
       </c>
       <c r="D68">
-        <v>142.9466011904768</v>
+        <v>134.2059718309705</v>
       </c>
       <c r="E68">
-        <v>159.6537506558605</v>
+        <v>154.6295022703841</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -3423,39 +3423,39 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <v>0.8953538554731694</v>
+        <v>0.8679195745990232</v>
       </c>
       <c r="I68">
-        <v>1.582180327263746</v>
+        <v>1.557589502491472</v>
       </c>
       <c r="J68">
-        <v>1.634341731812601</v>
+        <v>1.622575794915018</v>
       </c>
       <c r="K68">
-        <v>320.2971547619063</v>
+        <v>314.2744366197099</v>
       </c>
       <c r="L68">
-        <v>506.7678571428572</v>
+        <v>489.5105633802817</v>
       </c>
       <c r="M68">
-        <v>45.5</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B69" s="3">
-        <v>44227</v>
+        <v>44206</v>
       </c>
       <c r="C69" t="s">
         <v>23</v>
       </c>
       <c r="D69">
-        <v>140.7582857142912</v>
+        <v>140.0087321428582</v>
       </c>
       <c r="E69">
-        <v>156.2508330880756</v>
+        <v>158.1917127966816</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -3464,39 +3464,39 @@
         <v>0</v>
       </c>
       <c r="H69">
-        <v>0.9008482254616106</v>
+        <v>0.8850573122171492</v>
       </c>
       <c r="I69">
-        <v>1.577623562626929</v>
+        <v>1.572346885360321</v>
       </c>
       <c r="J69">
-        <v>1.625842648218127</v>
+        <v>1.62920241028032</v>
       </c>
       <c r="K69">
-        <v>321.2949226190491</v>
+        <v>319.8102678571428</v>
       </c>
       <c r="L69">
-        <v>506.8824404761905</v>
+        <v>502.8526785714286</v>
       </c>
       <c r="M69">
-        <v>37.4</v>
+        <v>41.4</v>
       </c>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B70" s="3">
-        <v>44234</v>
+        <v>44213</v>
       </c>
       <c r="C70" t="s">
         <v>23</v>
       </c>
       <c r="D70">
-        <v>139.5269047619021</v>
+        <v>144.4008035714284</v>
       </c>
       <c r="E70">
-        <v>158.8133813987119</v>
+        <v>161.2506918173763</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -3505,39 +3505,39 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>0.8785588691144999</v>
+        <v>0.8955050173364142</v>
       </c>
       <c r="I70">
-        <v>1.499982204354249</v>
+        <v>1.495412542330898</v>
       </c>
       <c r="J70">
-        <v>1.559982382773357</v>
+        <v>1.548066889717883</v>
       </c>
       <c r="K70">
-        <v>321.4403214285682</v>
+        <v>320.0094404761912</v>
       </c>
       <c r="L70">
-        <v>482.1547619047619</v>
+        <v>478.546130952381</v>
       </c>
       <c r="M70">
-        <v>41</v>
+        <v>47.6</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B71" s="3">
-        <v>44241</v>
+        <v>44220</v>
       </c>
       <c r="C71" t="s">
         <v>23</v>
       </c>
       <c r="D71">
-        <v>147.3453333333323</v>
+        <v>142.9466011904768</v>
       </c>
       <c r="E71">
-        <v>162.368476112245</v>
+        <v>159.6537506558605</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -3546,39 +3546,39 @@
         <v>0</v>
       </c>
       <c r="H71">
-        <v>0.907475002915423</v>
+        <v>0.8953538554731694</v>
       </c>
       <c r="I71">
-        <v>1.593994328535834</v>
+        <v>1.582180327263746</v>
       </c>
       <c r="J71">
-        <v>1.640668843431421</v>
+        <v>1.634341731812601</v>
       </c>
       <c r="K71">
-        <v>321.8703571428556</v>
+        <v>320.2971547619063</v>
       </c>
       <c r="L71">
-        <v>513.0595238095239</v>
+        <v>506.7678571428572</v>
       </c>
       <c r="M71">
-        <v>49.4</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B72" s="3">
-        <v>44248</v>
+        <v>44227</v>
       </c>
       <c r="C72" t="s">
         <v>23</v>
       </c>
       <c r="D72">
-        <v>145.3112023809559</v>
+        <v>140.7582857142912</v>
       </c>
       <c r="E72">
-        <v>157.4694775649883</v>
+        <v>156.2508330880756</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -3587,39 +3587,39 @@
         <v>0</v>
       </c>
       <c r="H72">
-        <v>0.9227896391602962</v>
+        <v>0.9008482254616106</v>
       </c>
       <c r="I72">
-        <v>1.593291214306311</v>
+        <v>1.577623562626929</v>
       </c>
       <c r="J72">
-        <v>1.630825206214054</v>
+        <v>1.625842648218127</v>
       </c>
       <c r="K72">
-        <v>323.9270476190529</v>
+        <v>321.2949226190491</v>
       </c>
       <c r="L72">
-        <v>516.110119047619</v>
+        <v>506.8824404761905</v>
       </c>
       <c r="M72">
-        <v>38.4</v>
+        <v>37.4</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B73" s="3">
-        <v>44255</v>
+        <v>44234</v>
       </c>
       <c r="C73" t="s">
         <v>23</v>
       </c>
       <c r="D73">
-        <v>144.4887559523784</v>
+        <v>139.5269047619021</v>
       </c>
       <c r="E73">
-        <v>156.9040522203854</v>
+        <v>158.8133813987119</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -3628,39 +3628,39 @@
         <v>0</v>
       </c>
       <c r="H73">
-        <v>0.9208733229491823</v>
+        <v>0.8785588691144999</v>
       </c>
       <c r="I73">
-        <v>1.591420056288376</v>
+        <v>1.499982204354249</v>
       </c>
       <c r="J73">
-        <v>1.629557999065331</v>
+        <v>1.559982382773357</v>
       </c>
       <c r="K73">
-        <v>325.5366011904719</v>
+        <v>321.4403214285682</v>
       </c>
       <c r="L73">
-        <v>518.0654761904761</v>
+        <v>482.1547619047619</v>
       </c>
       <c r="M73">
-        <v>36.2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B74" s="3">
-        <v>44262</v>
+        <v>44241</v>
       </c>
       <c r="C74" t="s">
         <v>23</v>
       </c>
       <c r="D74">
-        <v>144.8991190476143</v>
+        <v>147.3453333333323</v>
       </c>
       <c r="E74">
-        <v>157.7356201769991</v>
+        <v>162.368476112245</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -3669,39 +3669,39 @@
         <v>0</v>
       </c>
       <c r="H74">
-        <v>0.918620149874958</v>
+        <v>0.907475002915423</v>
       </c>
       <c r="I74">
-        <v>1.585400082593668</v>
+        <v>1.593994328535834</v>
       </c>
       <c r="J74">
-        <v>1.624620555810425</v>
+        <v>1.640668843431421</v>
       </c>
       <c r="K74">
-        <v>327.2908273809534</v>
+        <v>321.8703571428556</v>
       </c>
       <c r="L74">
-        <v>518.8869047619048</v>
+        <v>513.0595238095239</v>
       </c>
       <c r="M74">
-        <v>34.7</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B75" s="3">
-        <v>44269</v>
+        <v>44248</v>
       </c>
       <c r="C75" t="s">
         <v>23</v>
       </c>
       <c r="D75">
-        <v>150.2623095238093</v>
+        <v>145.3112023809559</v>
       </c>
       <c r="E75">
-        <v>947.880581257889</v>
+        <v>157.4694775649883</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -3710,39 +3710,39 @@
         <v>0</v>
       </c>
       <c r="H75">
-        <v>0.158524515107592</v>
+        <v>0.9227896391602962</v>
       </c>
       <c r="I75">
-        <v>0.2211518480156466</v>
+        <v>1.593291214306311</v>
       </c>
       <c r="J75">
-        <v>0.5821255774800674</v>
+        <v>1.630825206214054</v>
       </c>
       <c r="K75">
-        <v>2209.629694985043</v>
+        <v>323.9270476190529</v>
       </c>
       <c r="L75">
-        <v>488.6636904761905</v>
+        <v>516.110119047619</v>
       </c>
       <c r="M75">
-        <v>45.4</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B76" s="3">
-        <v>44276</v>
+        <v>44255</v>
       </c>
       <c r="C76" t="s">
         <v>23</v>
       </c>
       <c r="D76">
-        <v>152.0430000000023</v>
+        <v>144.4887559523784</v>
       </c>
       <c r="E76">
-        <v>2518.536252145573</v>
+        <v>156.9040522203854</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3751,39 +3751,39 @@
         <v>0</v>
       </c>
       <c r="H76">
-        <v>0.06036958962590869</v>
+        <v>0.9208733229491823</v>
       </c>
       <c r="I76">
-        <v>0.08316071538262837</v>
+        <v>1.591420056288376</v>
       </c>
       <c r="J76">
-        <v>0.4786756228728111</v>
+        <v>1.629557999065331</v>
       </c>
       <c r="K76">
-        <v>5983.322517885898</v>
+        <v>325.5366011904719</v>
       </c>
       <c r="L76">
-        <v>497.577380952381</v>
+        <v>518.0654761904761</v>
       </c>
       <c r="M76">
-        <v>42.6</v>
+        <v>36.2</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B77" s="3">
-        <v>44283</v>
+        <v>44262</v>
       </c>
       <c r="C77" t="s">
         <v>23</v>
       </c>
       <c r="D77">
-        <v>141.0593869047672</v>
+        <v>144.8991190476143</v>
       </c>
       <c r="E77">
-        <v>2505.677077193588</v>
+        <v>157.7356201769991</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -3792,39 +3792,39 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>0.05629591625699698</v>
+        <v>0.918620149874958</v>
       </c>
       <c r="I77">
-        <v>0.08560584577700275</v>
+        <v>1.585400082593668</v>
       </c>
       <c r="J77">
-        <v>0.481369956044975</v>
+        <v>1.624620555810425</v>
       </c>
       <c r="K77">
-        <v>5974.815878801474</v>
+        <v>327.2908273809534</v>
       </c>
       <c r="L77">
-        <v>511.4791666666667</v>
+        <v>518.8869047619048</v>
       </c>
       <c r="M77">
-        <v>23.1</v>
+        <v>34.7</v>
       </c>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B78" s="3">
-        <v>44290</v>
+        <v>44269</v>
       </c>
       <c r="C78" t="s">
         <v>23</v>
       </c>
       <c r="D78">
-        <v>156.4540059523757</v>
+        <v>150.2623095238093</v>
       </c>
       <c r="E78">
-        <v>2498.594875371729</v>
+        <v>947.880581257889</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -3833,39 +3833,39 @@
         <v>0</v>
       </c>
       <c r="H78">
-        <v>0.06261679614191124</v>
+        <v>0.158524515107592</v>
       </c>
       <c r="I78">
-        <v>0.08992120805352749</v>
+        <v>0.2211518480156466</v>
       </c>
       <c r="J78">
-        <v>0.4835812761090927</v>
+        <v>0.5821255774800674</v>
       </c>
       <c r="K78">
-        <v>5949.653163929142</v>
+        <v>2209.629694985043</v>
       </c>
       <c r="L78">
-        <v>535</v>
+        <v>488.6636904761905</v>
       </c>
       <c r="M78">
-        <v>30.3</v>
+        <v>45.4</v>
       </c>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B79" s="3">
-        <v>44297</v>
+        <v>44276</v>
       </c>
       <c r="C79" t="s">
         <v>23</v>
       </c>
       <c r="D79">
-        <v>158.7145476190518</v>
+        <v>152.0430000000023</v>
       </c>
       <c r="E79">
-        <v>2501.366705243571</v>
+        <v>2518.536252145573</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3874,39 +3874,39 @@
         <v>0</v>
       </c>
       <c r="H79">
-        <v>0.06345113144999541</v>
+        <v>0.06036958962590869</v>
       </c>
       <c r="I79">
-        <v>0.09059327195653993</v>
+        <v>0.08316071538262837</v>
       </c>
       <c r="J79">
-        <v>0.4836870519675929</v>
+        <v>0.4786756228728111</v>
       </c>
       <c r="K79">
-        <v>5959.52486848977</v>
+        <v>5983.322517885898</v>
       </c>
       <c r="L79">
-        <v>539.8928571428571</v>
+        <v>497.577380952381</v>
       </c>
       <c r="M79">
-        <v>27.3</v>
+        <v>42.6</v>
       </c>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B80" s="3">
-        <v>44304</v>
+        <v>44283</v>
       </c>
       <c r="C80" t="s">
         <v>23</v>
       </c>
       <c r="D80">
-        <v>156.8428750000007</v>
+        <v>141.0593869047672</v>
       </c>
       <c r="E80">
-        <v>734.8431290413783</v>
+        <v>2505.677077193588</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -3915,39 +3915,39 @@
         <v>0</v>
       </c>
       <c r="H80">
-        <v>0.2134372205461134</v>
+        <v>0.05629591625699698</v>
       </c>
       <c r="I80">
-        <v>0.8809602459572561</v>
+        <v>0.08560584577700275</v>
       </c>
       <c r="J80">
-        <v>1.216479171086076</v>
+        <v>0.481369956044975</v>
       </c>
       <c r="K80">
-        <v>1722.705369956287</v>
+        <v>5974.815878801474</v>
       </c>
       <c r="L80">
-        <v>1517.634946428572</v>
+        <v>511.4791666666667</v>
       </c>
       <c r="M80">
-        <v>29.5</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B81" s="3">
-        <v>44311</v>
+        <v>44290</v>
       </c>
       <c r="C81" t="s">
         <v>23</v>
       </c>
       <c r="D81">
-        <v>156.0972083333292</v>
+        <v>156.4540059523757</v>
       </c>
       <c r="E81">
-        <v>150.7338867132495</v>
+        <v>2498.594875371729</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -3956,39 +3956,39 @@
         <v>0</v>
       </c>
       <c r="H81">
-        <v>1.0355813927248</v>
+        <v>0.06261679614191124</v>
       </c>
       <c r="I81">
-        <v>1.587780193108647</v>
+        <v>0.08992120805352749</v>
       </c>
       <c r="J81">
-        <v>1.571770199879942</v>
+        <v>0.4835812761090927</v>
       </c>
       <c r="K81">
-        <v>334.9983690476233</v>
+        <v>5949.653163929142</v>
       </c>
       <c r="L81">
-        <v>531.9037750975085</v>
+        <v>535</v>
       </c>
       <c r="M81">
-        <v>18.7</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B82" s="3">
-        <v>44318</v>
+        <v>44297</v>
       </c>
       <c r="C82" t="s">
         <v>23</v>
       </c>
       <c r="D82">
-        <v>153.5751964285737</v>
+        <v>158.7145476190518</v>
       </c>
       <c r="E82">
-        <v>152.6345617785694</v>
+        <v>2501.366705243571</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -3997,39 +3997,39 @@
         <v>0</v>
       </c>
       <c r="H82">
-        <v>1.006162658306504</v>
+        <v>0.06345113144999541</v>
       </c>
       <c r="I82">
-        <v>1.570878098096148</v>
+        <v>0.09059327195653993</v>
       </c>
       <c r="J82">
-        <v>1.568110925363815</v>
+        <v>0.4836870519675929</v>
       </c>
       <c r="K82">
-        <v>339.926250000002</v>
+        <v>5959.52486848977</v>
       </c>
       <c r="L82">
-        <v>533.9827010929678</v>
+        <v>539.8928571428571</v>
       </c>
       <c r="M82">
-        <v>19.3</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B83" s="3">
-        <v>44325</v>
+        <v>44304</v>
       </c>
       <c r="C83" t="s">
         <v>23</v>
       </c>
       <c r="D83">
-        <v>152.6765714285651</v>
+        <v>156.8428750000007</v>
       </c>
       <c r="E83">
-        <v>150.6232778977588</v>
+        <v>734.8431290413783</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -4038,39 +4038,39 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>1.013631980125941</v>
+        <v>0.2134372205461134</v>
       </c>
       <c r="I83">
-        <v>1.558810470238923</v>
+        <v>0.8809602459572561</v>
       </c>
       <c r="J83">
-        <v>1.552784212443288</v>
+        <v>1.216479171086076</v>
       </c>
       <c r="K83">
-        <v>340.7244761904724</v>
+        <v>1722.705369956287</v>
       </c>
       <c r="L83">
-        <v>531.124880952381</v>
+        <v>1517.634946428572</v>
       </c>
       <c r="M83">
-        <v>13.6</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B84" s="3">
-        <v>44332</v>
+        <v>44311</v>
       </c>
       <c r="C84" t="s">
         <v>23</v>
       </c>
       <c r="D84">
-        <v>157.3976964285775</v>
+        <v>156.0972083333292</v>
       </c>
       <c r="E84">
-        <v>154.2539879165841</v>
+        <v>150.7338867132495</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -4079,39 +4079,39 @@
         <v>0</v>
       </c>
       <c r="H84">
-        <v>1.020380079338328</v>
+        <v>1.0355813927248</v>
       </c>
       <c r="I84">
-        <v>1.570803371983793</v>
+        <v>1.587780193108647</v>
       </c>
       <c r="J84">
-        <v>1.561632169622951</v>
+        <v>1.571770199879942</v>
       </c>
       <c r="K84">
-        <v>342.7804107142867</v>
+        <v>334.9983690476233</v>
       </c>
       <c r="L84">
-        <v>538.4406250000001</v>
+        <v>531.9037750975085</v>
       </c>
       <c r="M84">
-        <v>20.4</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B85" s="3">
-        <v>44339</v>
+        <v>44318</v>
       </c>
       <c r="C85" t="s">
         <v>23</v>
       </c>
       <c r="D85">
-        <v>150.4058869047634</v>
+        <v>153.5751964285737</v>
       </c>
       <c r="E85">
-        <v>149.8152226645259</v>
+        <v>152.6345617785694</v>
       </c>
       <c r="F85">
         <v>0</v>
@@ -4120,39 +4120,39 @@
         <v>0</v>
       </c>
       <c r="H85">
-        <v>1.003942618311626</v>
+        <v>1.006162658306504</v>
       </c>
       <c r="I85">
-        <v>1.560848303349736</v>
+        <v>1.570878098096148</v>
       </c>
       <c r="J85">
-        <v>1.559123387974313</v>
+        <v>1.568110925363815</v>
       </c>
       <c r="K85">
-        <v>342.4308511904729</v>
+        <v>339.926250000002</v>
       </c>
       <c r="L85">
-        <v>534.4826130952381</v>
+        <v>533.9827010929678</v>
       </c>
       <c r="M85">
-        <v>12</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B86" s="3">
-        <v>44346</v>
+        <v>44325</v>
       </c>
       <c r="C86" t="s">
         <v>23</v>
       </c>
       <c r="D86">
-        <v>150.0719345238093</v>
+        <v>152.6765714285651</v>
       </c>
       <c r="E86">
-        <v>148.9184643458958</v>
+        <v>150.6232778977588</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -4161,39 +4161,39 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <v>1.007745649157611</v>
+        <v>1.013631980125941</v>
       </c>
       <c r="I86">
-        <v>1.547534877460135</v>
+        <v>1.558810470238923</v>
       </c>
       <c r="J86">
-        <v>1.544166545805853</v>
+        <v>1.552784212443288</v>
       </c>
       <c r="K86">
-        <v>342.4455476190529</v>
+        <v>340.7244761904724</v>
       </c>
       <c r="L86">
-        <v>529.9464285714286</v>
+        <v>531.124880952381</v>
       </c>
       <c r="M86">
-        <v>11.6</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="1">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B87" s="3">
-        <v>44353</v>
+        <v>44332</v>
       </c>
       <c r="C87" t="s">
         <v>23</v>
       </c>
       <c r="D87">
-        <v>152.2536964285675</v>
+        <v>157.3976964285775</v>
       </c>
       <c r="E87">
-        <v>145.6629314091923</v>
+        <v>154.2539879165841</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -4202,39 +4202,39 @@
         <v>0</v>
       </c>
       <c r="H87">
-        <v>1.045246686686956</v>
+        <v>1.020380079338328</v>
       </c>
       <c r="I87">
-        <v>1.559609421173874</v>
+        <v>1.570803371983793</v>
       </c>
       <c r="J87">
-        <v>1.540464493763287</v>
+        <v>1.561632169622951</v>
       </c>
       <c r="K87">
-        <v>344.256464285715</v>
+        <v>342.7804107142867</v>
       </c>
       <c r="L87">
-        <v>536.905625</v>
+        <v>538.4406250000001</v>
       </c>
       <c r="M87">
-        <v>2.9</v>
+        <v>20.4</v>
       </c>
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B88" s="3">
-        <v>44360</v>
+        <v>44339</v>
       </c>
       <c r="C88" t="s">
         <v>23</v>
       </c>
       <c r="D88">
-        <v>157.0354821428634</v>
+        <v>150.4058869047634</v>
       </c>
       <c r="E88">
-        <v>151.1502679938704</v>
+        <v>149.8152226645259</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -4243,39 +4243,39 @@
         <v>0</v>
       </c>
       <c r="H88">
-        <v>1.038936180710125</v>
+        <v>1.003942618311626</v>
       </c>
       <c r="I88">
-        <v>1.569419507488795</v>
+        <v>1.560848303349736</v>
       </c>
       <c r="J88">
-        <v>1.55264447743385</v>
+        <v>1.559123387974313</v>
       </c>
       <c r="K88">
-        <v>350.8318095238092</v>
+        <v>342.4308511904729</v>
       </c>
       <c r="L88">
-        <v>550.6022857142857</v>
+        <v>534.4826130952381</v>
       </c>
       <c r="M88">
-        <v>7.9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B89" s="3">
-        <v>44367</v>
+        <v>44346</v>
       </c>
       <c r="C89" t="s">
         <v>23</v>
       </c>
       <c r="D89">
-        <v>151.8791547618984</v>
+        <v>150.0719345238093</v>
       </c>
       <c r="E89">
-        <v>151.3772036866484</v>
+        <v>148.9184643458958</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -4284,39 +4284,39 @@
         <v>0</v>
       </c>
       <c r="H89">
-        <v>1.003315896073025</v>
+        <v>1.007745649157611</v>
       </c>
       <c r="I89">
-        <v>1.548852670984837</v>
+        <v>1.547534877460135</v>
       </c>
       <c r="J89">
-        <v>1.547412523362798</v>
+        <v>1.544166545805853</v>
       </c>
       <c r="K89">
-        <v>348.5414047619062</v>
+        <v>342.4455476190529</v>
       </c>
       <c r="L89">
-        <v>539.8392857142857</v>
+        <v>529.9464285714286</v>
       </c>
       <c r="M89">
-        <v>10.5</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B90" s="3">
-        <v>44374</v>
+        <v>44353</v>
       </c>
       <c r="C90" t="s">
         <v>23</v>
       </c>
       <c r="D90">
-        <v>148.30996428572</v>
+        <v>152.2536964285675</v>
       </c>
       <c r="E90">
-        <v>150.0558700498584</v>
+        <v>145.6629314091923</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -4325,39 +4325,39 @@
         <v>0</v>
       </c>
       <c r="H90">
-        <v>0.9883649619067998</v>
+        <v>1.045246686686956</v>
       </c>
       <c r="I90">
-        <v>1.535492302740842</v>
+        <v>1.559609421173874</v>
       </c>
       <c r="J90">
-        <v>1.540533026392636</v>
+        <v>1.540464493763287</v>
       </c>
       <c r="K90">
-        <v>346.3601428571412</v>
+        <v>344.256464285715</v>
       </c>
       <c r="L90">
-        <v>531.8333333333334</v>
+        <v>536.905625</v>
       </c>
       <c r="M90">
-        <v>8.800000000000001</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B91" s="3">
-        <v>44381</v>
+        <v>44360</v>
       </c>
       <c r="C91" t="s">
         <v>23</v>
       </c>
       <c r="D91">
-        <v>158.1438511904728</v>
+        <v>157.0354821428634</v>
       </c>
       <c r="E91">
-        <v>152.5077765011403</v>
+        <v>151.1502679938704</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -4366,39 +4366,39 @@
         <v>0</v>
       </c>
       <c r="H91">
-        <v>1.036955982302255</v>
+        <v>1.038936180710125</v>
       </c>
       <c r="I91">
-        <v>1.56272533373313</v>
+        <v>1.569419507488795</v>
       </c>
       <c r="J91">
-        <v>1.546492552225222</v>
+        <v>1.55264447743385</v>
       </c>
       <c r="K91">
-        <v>347.2032619047566</v>
+        <v>350.8318095238092</v>
       </c>
       <c r="L91">
-        <v>542.5833333333334</v>
+        <v>550.6022857142857</v>
       </c>
       <c r="M91">
-        <v>14.4</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="1">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B92" s="3">
-        <v>44388</v>
+        <v>44367</v>
       </c>
       <c r="C92" t="s">
         <v>23</v>
       </c>
       <c r="D92">
-        <v>144.3952142857126</v>
+        <v>151.8791547618984</v>
       </c>
       <c r="E92">
-        <v>147.5998250432984</v>
+        <v>151.3772036866484</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -4407,39 +4407,39 @@
         <v>0</v>
       </c>
       <c r="H92">
-        <v>0.9782885192672436</v>
+        <v>1.003315896073025</v>
       </c>
       <c r="I92">
-        <v>1.525146884594245</v>
+        <v>1.548852670984837</v>
       </c>
       <c r="J92">
-        <v>1.534388991885071</v>
+        <v>1.547412523362798</v>
       </c>
       <c r="K92">
-        <v>346.7402678571442</v>
+        <v>348.5414047619062</v>
       </c>
       <c r="L92">
-        <v>528.8298392857143</v>
+        <v>539.8392857142857</v>
       </c>
       <c r="M92">
-        <v>5.2</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B93" s="3">
-        <v>44395</v>
+        <v>44374</v>
       </c>
       <c r="C93" t="s">
         <v>23</v>
       </c>
       <c r="D93">
-        <v>145.9704999999986</v>
+        <v>148.30996428572</v>
       </c>
       <c r="E93">
-        <v>147.1306517031884</v>
+        <v>150.0558700498584</v>
       </c>
       <c r="F93">
         <v>0</v>
@@ -4448,39 +4448,39 @@
         <v>0</v>
       </c>
       <c r="H93">
-        <v>0.9921148197893515</v>
+        <v>0.9883649619067998</v>
       </c>
       <c r="I93">
-        <v>1.530192496413252</v>
+        <v>1.535492302740842</v>
       </c>
       <c r="J93">
-        <v>1.533538840451344</v>
+        <v>1.540533026392636</v>
       </c>
       <c r="K93">
-        <v>346.6922976190468</v>
+        <v>346.3601428571412</v>
       </c>
       <c r="L93">
-        <v>530.5059523809524</v>
+        <v>531.8333333333334</v>
       </c>
       <c r="M93">
-        <v>4.6</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B94" s="3">
-        <v>44402</v>
+        <v>44381</v>
       </c>
       <c r="C94" t="s">
         <v>23</v>
       </c>
       <c r="D94">
-        <v>137.1910416666707</v>
+        <v>158.1438511904728</v>
       </c>
       <c r="E94">
-        <v>146.5751301568946</v>
+        <v>152.5077765011403</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -4489,39 +4489,39 @@
         <v>0</v>
       </c>
       <c r="H94">
-        <v>0.9359776213046564</v>
+        <v>1.036955982302255</v>
       </c>
       <c r="I94">
-        <v>1.508090070702715</v>
+        <v>1.56272533373313</v>
       </c>
       <c r="J94">
-        <v>1.535146361680138</v>
+        <v>1.546492552225222</v>
       </c>
       <c r="K94">
-        <v>346.8357321428567</v>
+        <v>347.2032619047566</v>
       </c>
       <c r="L94">
-        <v>523.0595238095239</v>
+        <v>542.5833333333334</v>
       </c>
       <c r="M94">
-        <v>2.8</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B95" s="3">
-        <v>44409</v>
+        <v>44388</v>
       </c>
       <c r="C95" t="s">
         <v>23</v>
       </c>
       <c r="D95">
-        <v>148.550464285715</v>
+        <v>144.3952142857126</v>
       </c>
       <c r="E95">
-        <v>149.5998146687054</v>
+        <v>147.5998250432984</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -4530,39 +4530,39 @@
         <v>0</v>
       </c>
       <c r="H95">
-        <v>0.9929856170924126</v>
+        <v>0.9782885192672436</v>
       </c>
       <c r="I95">
-        <v>1.543056571904535</v>
+        <v>1.525146884594245</v>
       </c>
       <c r="J95">
-        <v>1.546062060544356</v>
+        <v>1.534388991885071</v>
       </c>
       <c r="K95">
-        <v>349.1446845238097</v>
+        <v>346.7402678571442</v>
       </c>
       <c r="L95">
-        <v>538.75</v>
+        <v>528.8298392857143</v>
       </c>
       <c r="M95">
-        <v>6.5</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B96" s="3">
-        <v>44416</v>
+        <v>44395</v>
       </c>
       <c r="C96" t="s">
         <v>23</v>
       </c>
       <c r="D96">
-        <v>148.1289345238058</v>
+        <v>145.9704999999986</v>
       </c>
       <c r="E96">
-        <v>151.1467922160408</v>
+        <v>147.1306517031884</v>
       </c>
       <c r="F96">
         <v>0</v>
@@ -4571,39 +4571,39 @@
         <v>0</v>
       </c>
       <c r="H96">
-        <v>0.9800335974850102</v>
+        <v>0.9921148197893515</v>
       </c>
       <c r="I96">
-        <v>1.543234943406895</v>
+        <v>1.530192496413252</v>
       </c>
       <c r="J96">
-        <v>1.55184034428612</v>
+        <v>1.533538840451344</v>
       </c>
       <c r="K96">
-        <v>350.6934464285704</v>
+        <v>346.6922976190468</v>
       </c>
       <c r="L96">
-        <v>541.202380952381</v>
+        <v>530.5059523809524</v>
       </c>
       <c r="M96">
-        <v>8.800000000000001</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B97" s="3">
-        <v>44423</v>
+        <v>44402</v>
       </c>
       <c r="C97" t="s">
         <v>23</v>
       </c>
       <c r="D97">
-        <v>148.7178750000007</v>
+        <v>137.1910416666707</v>
       </c>
       <c r="E97">
-        <v>150.0896963079265</v>
+        <v>146.5751301568946</v>
       </c>
       <c r="F97">
         <v>0</v>
@@ -4612,39 +4612,39 @@
         <v>0</v>
       </c>
       <c r="H97">
-        <v>0.9908599901147686</v>
+        <v>0.9359776213046564</v>
       </c>
       <c r="I97">
-        <v>1.551949716378851</v>
+        <v>1.508090070702715</v>
       </c>
       <c r="J97">
-        <v>1.55584716173332</v>
+        <v>1.535146361680138</v>
       </c>
       <c r="K97">
-        <v>351.9796130952392</v>
+        <v>346.8357321428567</v>
       </c>
       <c r="L97">
-        <v>546.2546607142857</v>
+        <v>523.0595238095239</v>
       </c>
       <c r="M97">
-        <v>5.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B98" s="3">
-        <v>44430</v>
+        <v>44409</v>
       </c>
       <c r="C98" t="s">
         <v>23</v>
       </c>
       <c r="D98">
-        <v>149.8686607142833</v>
+        <v>148.550464285715</v>
       </c>
       <c r="E98">
-        <v>151.7328174491492</v>
+        <v>149.5998146687054</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -4653,19 +4653,19 @@
         <v>0</v>
       </c>
       <c r="H98">
-        <v>0.9877142152488488</v>
+        <v>0.9929856170924126</v>
       </c>
       <c r="I98">
-        <v>1.545537786875197</v>
+        <v>1.543056571904535</v>
       </c>
       <c r="J98">
-        <v>1.550819466275676</v>
+        <v>1.546062060544356</v>
       </c>
       <c r="K98">
-        <v>352.9477261904782</v>
+        <v>349.1446845238097</v>
       </c>
       <c r="L98">
-        <v>545.4940476190476</v>
+        <v>538.75</v>
       </c>
       <c r="M98">
         <v>6.5</v>
@@ -4673,19 +4673,19 @@
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B99" s="3">
-        <v>44437</v>
+        <v>44416</v>
       </c>
       <c r="C99" t="s">
         <v>23</v>
       </c>
       <c r="D99">
-        <v>153.2249880952406</v>
+        <v>148.1289345238058</v>
       </c>
       <c r="E99">
-        <v>155.9768625214436</v>
+        <v>151.1467922160408</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -4694,39 +4694,39 @@
         <v>0</v>
       </c>
       <c r="H99">
-        <v>0.9823571625834909</v>
+        <v>0.9800335974850102</v>
       </c>
       <c r="I99">
-        <v>1.548289623279574</v>
+        <v>1.543234943406895</v>
       </c>
       <c r="J99">
-        <v>1.556088679369513</v>
+        <v>1.55184034428612</v>
       </c>
       <c r="K99">
-        <v>352.847113095235</v>
+        <v>350.6934464285704</v>
       </c>
       <c r="L99">
-        <v>546.3095238095239</v>
+        <v>541.202380952381</v>
       </c>
       <c r="M99">
-        <v>15.6</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B100" s="3">
-        <v>44444</v>
+        <v>44423</v>
       </c>
       <c r="C100" t="s">
         <v>23</v>
       </c>
       <c r="D100">
-        <v>154.2299345238079</v>
+        <v>148.7178750000007</v>
       </c>
       <c r="E100">
-        <v>154.96937297445</v>
+        <v>150.0896963079265</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -4735,39 +4735,39 @@
         <v>0</v>
       </c>
       <c r="H100">
-        <v>0.9952284865296315</v>
+        <v>0.9908599901147686</v>
       </c>
       <c r="I100">
-        <v>1.541009956893704</v>
+        <v>1.551949716378851</v>
       </c>
       <c r="J100">
-        <v>1.5430874983344</v>
+        <v>1.55584716173332</v>
       </c>
       <c r="K100">
-        <v>355.9199523809532</v>
+        <v>351.9796130952392</v>
       </c>
       <c r="L100">
-        <v>548.4761904761905</v>
+        <v>546.2546607142857</v>
       </c>
       <c r="M100">
-        <v>11.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B101" s="3">
-        <v>44451</v>
+        <v>44430</v>
       </c>
       <c r="C101" t="s">
         <v>23</v>
       </c>
       <c r="D101">
-        <v>150.5623452380976</v>
+        <v>149.8686607142833</v>
       </c>
       <c r="E101">
-        <v>153.8068462561213</v>
+        <v>151.7328174491492</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -4776,39 +4776,39 @@
         <v>0</v>
       </c>
       <c r="H101">
-        <v>0.9789053537147435</v>
+        <v>0.9877142152488488</v>
       </c>
       <c r="I101">
-        <v>1.531794692153567</v>
+        <v>1.545537786875197</v>
       </c>
       <c r="J101">
-        <v>1.540912275430181</v>
+        <v>1.550819466275676</v>
       </c>
       <c r="K101">
-        <v>355.8509880952437</v>
+        <v>352.9477261904782</v>
       </c>
       <c r="L101">
-        <v>545.0906547619048</v>
+        <v>545.4940476190476</v>
       </c>
       <c r="M101">
-        <v>8.9</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B102" s="3">
-        <v>44458</v>
+        <v>44437</v>
       </c>
       <c r="C102" t="s">
         <v>23</v>
       </c>
       <c r="D102">
-        <v>158.337166666663</v>
+        <v>153.2249880952406</v>
       </c>
       <c r="E102">
-        <v>154.8723022349019</v>
+        <v>155.9768625214436</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -4817,39 +4817,39 @@
         <v>0</v>
       </c>
       <c r="H102">
-        <v>1.02237239572061</v>
+        <v>0.9823571625834909</v>
       </c>
       <c r="I102">
-        <v>1.551825866658735</v>
+        <v>1.548289623279574</v>
       </c>
       <c r="J102">
-        <v>1.542091360166521</v>
+        <v>1.556088679369513</v>
       </c>
       <c r="K102">
-        <v>355.9363214285667</v>
+        <v>352.847113095235</v>
       </c>
       <c r="L102">
-        <v>552.3511904761905</v>
+        <v>546.3095238095239</v>
       </c>
       <c r="M102">
-        <v>11.2</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B103" s="3">
-        <v>44465</v>
+        <v>44444</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
       </c>
       <c r="D103">
-        <v>155.2170833333373</v>
+        <v>154.2299345238079</v>
       </c>
       <c r="E103">
-        <v>155.1062633025237</v>
+        <v>154.96937297445</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -4858,39 +4858,39 @@
         <v>0</v>
       </c>
       <c r="H103">
-        <v>1.00071447811619</v>
+        <v>0.9952284865296315</v>
       </c>
       <c r="I103">
-        <v>1.541391284642335</v>
+        <v>1.541009956893704</v>
       </c>
       <c r="J103">
-        <v>1.541081335502792</v>
+        <v>1.5430874983344</v>
       </c>
       <c r="K103">
-        <v>357.5426309523783</v>
+        <v>355.9199523809532</v>
       </c>
       <c r="L103">
-        <v>551.1130952380952</v>
+        <v>548.4761904761905</v>
       </c>
       <c r="M103">
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="1">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B104" s="3">
-        <v>44472</v>
+        <v>44451</v>
       </c>
       <c r="C104" t="s">
         <v>23</v>
       </c>
       <c r="D104">
-        <v>150.4812380952339</v>
+        <v>150.5623452380976</v>
       </c>
       <c r="E104">
-        <v>158.2787981330455</v>
+        <v>153.8068462561213</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -4899,39 +4899,39 @@
         <v>0</v>
       </c>
       <c r="H104">
-        <v>0.9507352840065342</v>
+        <v>0.9789053537147435</v>
       </c>
       <c r="I104">
-        <v>1.524838044019881</v>
+        <v>1.531794692153567</v>
       </c>
       <c r="J104">
-        <v>1.546492345788618</v>
+        <v>1.540912275430181</v>
       </c>
       <c r="K104">
-        <v>360.0928869047646</v>
+        <v>355.8509880952437</v>
       </c>
       <c r="L104">
-        <v>549.0833333333334</v>
+        <v>545.0906547619048</v>
       </c>
       <c r="M104">
-        <v>14.8</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="1">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B105" s="3">
-        <v>44479</v>
+        <v>44458</v>
       </c>
       <c r="C105" t="s">
         <v>23</v>
       </c>
       <c r="D105">
-        <v>150.4646190476293</v>
+        <v>158.337166666663</v>
       </c>
       <c r="E105">
-        <v>155.9312647611605</v>
+        <v>154.8723022349019</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -4940,39 +4940,39 @@
         <v>0</v>
       </c>
       <c r="H105">
-        <v>0.9649419523281334</v>
+        <v>1.02237239572061</v>
       </c>
       <c r="I105">
-        <v>1.530703656965332</v>
+        <v>1.551825866658735</v>
       </c>
       <c r="J105">
-        <v>1.545841759963428</v>
+        <v>1.542091360166521</v>
       </c>
       <c r="K105">
-        <v>361.1182797619064</v>
+        <v>355.9363214285667</v>
       </c>
       <c r="L105">
-        <v>552.7650714285713</v>
+        <v>552.3511904761905</v>
       </c>
       <c r="M105">
-        <v>7.6</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="1">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B106" s="3">
-        <v>44486</v>
+        <v>44465</v>
       </c>
       <c r="C106" t="s">
         <v>23</v>
       </c>
       <c r="D106">
-        <v>154.9318988095259</v>
+        <v>155.2170833333373</v>
       </c>
       <c r="E106">
-        <v>161.2658054169062</v>
+        <v>155.1062633025237</v>
       </c>
       <c r="F106">
         <v>0</v>
@@ -4981,39 +4981,39 @@
         <v>0</v>
       </c>
       <c r="H106">
-        <v>0.9607238088012162</v>
+        <v>1.00071447811619</v>
       </c>
       <c r="I106">
-        <v>1.558349824050244</v>
+        <v>1.541391284642335</v>
       </c>
       <c r="J106">
-        <v>1.57583734875986</v>
+        <v>1.541081335502792</v>
       </c>
       <c r="K106">
-        <v>362.19572023809</v>
+        <v>357.5426309523783</v>
       </c>
       <c r="L106">
-        <v>564.4276369047618</v>
+        <v>551.1130952380952</v>
       </c>
       <c r="M106">
-        <v>18.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="1">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B107" s="3">
-        <v>44493</v>
+        <v>44472</v>
       </c>
       <c r="C107" t="s">
         <v>23</v>
       </c>
       <c r="D107">
-        <v>160.2658154761884</v>
+        <v>150.4812380952339</v>
       </c>
       <c r="E107">
-        <v>157.5998220198986</v>
+        <v>158.2787981330455</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -5022,39 +5022,39 @@
         <v>0</v>
       </c>
       <c r="H107">
-        <v>1.016916221237567</v>
+        <v>0.9507352840065342</v>
       </c>
       <c r="I107">
-        <v>1.562263884482379</v>
+        <v>1.524838044019881</v>
       </c>
       <c r="J107">
-        <v>1.554932809515883</v>
+        <v>1.546492345788618</v>
       </c>
       <c r="K107">
-        <v>363.656553571434</v>
+        <v>360.0928869047646</v>
       </c>
       <c r="L107">
-        <v>568.1274999999999</v>
+        <v>549.0833333333334</v>
       </c>
       <c r="M107">
-        <v>10.5</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="1">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B108" s="3">
-        <v>44500</v>
+        <v>44479</v>
       </c>
       <c r="C108" t="s">
         <v>23</v>
       </c>
       <c r="D108">
-        <v>166.2139940476156</v>
+        <v>150.4646190476293</v>
       </c>
       <c r="E108">
-        <v>157.8899805313582</v>
+        <v>155.9312647611605</v>
       </c>
       <c r="F108">
         <v>0</v>
@@ -5063,39 +5063,39 @@
         <v>0</v>
       </c>
       <c r="H108">
-        <v>1.052720340380333</v>
+        <v>0.9649419523281334</v>
       </c>
       <c r="I108">
-        <v>1.579345157025566</v>
+        <v>1.530703656965332</v>
       </c>
       <c r="J108">
-        <v>1.556560900646736</v>
+        <v>1.545841759963428</v>
       </c>
       <c r="K108">
-        <v>365.3405833333354</v>
+        <v>361.1182797619064</v>
       </c>
       <c r="L108">
-        <v>576.998880952381</v>
+        <v>552.7650714285713</v>
       </c>
       <c r="M108">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="1">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B109" s="3">
-        <v>44507</v>
+        <v>44486</v>
       </c>
       <c r="C109" t="s">
         <v>23</v>
       </c>
       <c r="D109">
-        <v>167.3687499999956</v>
+        <v>154.9318988095259</v>
       </c>
       <c r="E109">
-        <v>164.4964293230406</v>
+        <v>161.2658054169062</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -5104,39 +5104,39 @@
         <v>0</v>
       </c>
       <c r="H109">
-        <v>1.017461294988441</v>
+        <v>0.9607238088012162</v>
       </c>
       <c r="I109">
-        <v>1.577470453258754</v>
+        <v>1.558349824050244</v>
       </c>
       <c r="J109">
-        <v>1.569640210281676</v>
+        <v>1.57583734875986</v>
       </c>
       <c r="K109">
-        <v>366.8239523809503</v>
+        <v>362.19572023809</v>
       </c>
       <c r="L109">
-        <v>578.6539464285715</v>
+        <v>564.4276369047618</v>
       </c>
       <c r="M109">
-        <v>19.7</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B110" s="3">
-        <v>44514</v>
+        <v>44493</v>
       </c>
       <c r="C110" t="s">
         <v>23</v>
       </c>
       <c r="D110">
-        <v>167.1621369047623</v>
+        <v>160.2658154761884</v>
       </c>
       <c r="E110">
-        <v>163.8692706275791</v>
+        <v>157.5998220198986</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -5145,39 +5145,39 @@
         <v>0</v>
       </c>
       <c r="H110">
-        <v>1.020094470821603</v>
+        <v>1.016916221237567</v>
       </c>
       <c r="I110">
-        <v>1.587933394553531</v>
+        <v>1.562263884482379</v>
       </c>
       <c r="J110">
-        <v>1.578943403081213</v>
+        <v>1.554932809515883</v>
       </c>
       <c r="K110">
-        <v>366.2813571428525</v>
+        <v>363.656553571434</v>
       </c>
       <c r="L110">
-        <v>581.6303988095236</v>
+        <v>568.1274999999999</v>
       </c>
       <c r="M110">
-        <v>19.1</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B111" s="3">
-        <v>44521</v>
+        <v>44500</v>
       </c>
       <c r="C111" t="s">
         <v>23</v>
       </c>
       <c r="D111">
-        <v>164.4951964285713</v>
+        <v>166.2139940476156</v>
       </c>
       <c r="E111">
-        <v>165.0337284204268</v>
+        <v>157.8899805313582</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -5186,39 +5186,39 @@
         <v>0</v>
       </c>
       <c r="H111">
-        <v>0.9967368367847597</v>
+        <v>1.052720340380333</v>
       </c>
       <c r="I111">
-        <v>1.573310721672806</v>
+        <v>1.579345157025566</v>
       </c>
       <c r="J111">
-        <v>1.574762832595814</v>
+        <v>1.556560900646736</v>
       </c>
       <c r="K111">
-        <v>370.8614702381061</v>
+        <v>365.3405833333354</v>
       </c>
       <c r="L111">
-        <v>583.4803273809524</v>
+        <v>576.998880952381</v>
       </c>
       <c r="M111">
-        <v>17.9</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B112" s="3">
-        <v>44528</v>
+        <v>44507</v>
       </c>
       <c r="C112" t="s">
         <v>23</v>
       </c>
       <c r="D112">
-        <v>173.2202976190463</v>
+        <v>167.3687499999956</v>
       </c>
       <c r="E112">
-        <v>166.2821394826832</v>
+        <v>164.4964293230406</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -5227,39 +5227,39 @@
         <v>0</v>
       </c>
       <c r="H112">
-        <v>1.041725215696335</v>
+        <v>1.017461294988441</v>
       </c>
       <c r="I112">
-        <v>1.58316812519325</v>
+        <v>1.577470453258754</v>
       </c>
       <c r="J112">
-        <v>1.564573416394278</v>
+        <v>1.569640210281676</v>
       </c>
       <c r="K112">
-        <v>373.1253988095171</v>
+        <v>366.8239523809503</v>
       </c>
       <c r="L112">
-        <v>590.7202380952381</v>
+        <v>578.6539464285715</v>
       </c>
       <c r="M112">
-        <v>16.2</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="113" spans="1:13">
       <c r="A113" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B113" s="3">
-        <v>44535</v>
+        <v>44514</v>
       </c>
       <c r="C113" t="s">
         <v>23</v>
       </c>
       <c r="D113">
-        <v>175.1457976190528</v>
+        <v>167.1621369047623</v>
       </c>
       <c r="E113">
-        <v>175.3893679509762</v>
+        <v>163.8692706275791</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -5268,39 +5268,39 @@
         <v>0</v>
       </c>
       <c r="H113">
-        <v>0.9986112594237101</v>
+        <v>1.020094470821603</v>
       </c>
       <c r="I113">
-        <v>1.596230442639184</v>
+        <v>1.587933394553531</v>
       </c>
       <c r="J113">
-        <v>1.596879508498238</v>
+        <v>1.578943403081213</v>
       </c>
       <c r="K113">
-        <v>375.262892857144</v>
+        <v>366.2813571428525</v>
       </c>
       <c r="L113">
-        <v>599.0060535714285</v>
+        <v>581.6303988095236</v>
       </c>
       <c r="M113">
-        <v>30.7</v>
+        <v>19.1</v>
       </c>
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B114" s="3">
-        <v>44542</v>
+        <v>44521</v>
       </c>
       <c r="C114" t="s">
         <v>23</v>
       </c>
       <c r="D114">
-        <v>178.8955476190451</v>
+        <v>164.4951964285713</v>
       </c>
       <c r="E114">
-        <v>179.3276510694548</v>
+        <v>165.0337284204268</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -5309,39 +5309,39 @@
         <v>0</v>
       </c>
       <c r="H114">
-        <v>0.9975904248573336</v>
+        <v>0.9967368367847597</v>
       </c>
       <c r="I114">
-        <v>1.607968930666337</v>
+        <v>1.573310721672806</v>
       </c>
       <c r="J114">
-        <v>1.609123372266538</v>
+        <v>1.574762832595814</v>
       </c>
       <c r="K114">
-        <v>374.296499999994</v>
+        <v>370.8614702381061</v>
       </c>
       <c r="L114">
-        <v>601.8571428571429</v>
+        <v>583.4803273809524</v>
       </c>
       <c r="M114">
-        <v>41.4</v>
+        <v>17.9</v>
       </c>
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B115" s="3">
-        <v>44549</v>
+        <v>44528</v>
       </c>
       <c r="C115" t="s">
         <v>23</v>
       </c>
       <c r="D115">
-        <v>172.564595238095</v>
+        <v>173.2202976190463</v>
       </c>
       <c r="E115">
-        <v>172.5371725861211</v>
+        <v>166.2821394826832</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -5350,39 +5350,39 @@
         <v>0</v>
       </c>
       <c r="H115">
-        <v>1.00015893764551</v>
+        <v>1.041725215696335</v>
       </c>
       <c r="I115">
-        <v>1.579236706502634</v>
+        <v>1.58316812519325</v>
       </c>
       <c r="J115">
-        <v>1.579163589419889</v>
+        <v>1.564573416394278</v>
       </c>
       <c r="K115">
-        <v>375.0512321428673</v>
+        <v>373.1253988095171</v>
       </c>
       <c r="L115">
-        <v>592.2946726190477</v>
+        <v>590.7202380952381</v>
       </c>
       <c r="M115">
-        <v>27.9</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B116" s="3">
-        <v>44556</v>
+        <v>44535</v>
       </c>
       <c r="C116" t="s">
         <v>23</v>
       </c>
       <c r="D116">
-        <v>170.0147678571465</v>
+        <v>175.1457976190528</v>
       </c>
       <c r="E116">
-        <v>171.4509159512136</v>
+        <v>175.3893679509762</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -5391,470 +5391,716 @@
         <v>0</v>
       </c>
       <c r="H116">
-        <v>0.9916235612618378</v>
+        <v>0.9986112594237101</v>
       </c>
       <c r="I116">
-        <v>1.560486156660549</v>
+        <v>1.596230442639184</v>
       </c>
       <c r="J116">
-        <v>1.564317780166184</v>
+        <v>1.596879508498238</v>
       </c>
       <c r="K116">
-        <v>374.8145119047591</v>
+        <v>375.262892857144</v>
       </c>
       <c r="L116">
-        <v>584.8928571428571</v>
+        <v>599.0060535714285</v>
       </c>
       <c r="M116">
-        <v>24.7</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="1">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B117" s="3">
-        <v>44563</v>
+        <v>44542</v>
       </c>
       <c r="C117" t="s">
         <v>23</v>
       </c>
       <c r="D117">
-        <v>172.4510654761855</v>
+        <v>178.8955476190451</v>
       </c>
       <c r="E117">
-        <v>176.1123861937075</v>
+        <v>179.3276510694548</v>
       </c>
       <c r="F117">
-        <v>-3.661320717521988</v>
+        <v>0</v>
       </c>
       <c r="G117">
-        <v>-3.661320717521988</v>
+        <v>0</v>
       </c>
       <c r="H117">
-        <v>0.9792103167945559</v>
+        <v>0.9975904248573336</v>
       </c>
       <c r="I117">
-        <v>1.573893975160251</v>
+        <v>1.607968930666337</v>
       </c>
       <c r="J117">
-        <v>1.583661666017127</v>
+        <v>1.609123372266538</v>
       </c>
       <c r="K117">
-        <v>374.8399464285689</v>
+        <v>374.296499999994</v>
       </c>
       <c r="L117">
-        <v>589.9583333333334</v>
+        <v>601.8571428571429</v>
       </c>
       <c r="M117">
-        <v>32.6</v>
+        <v>41.4</v>
       </c>
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B118" s="3">
-        <v>44570</v>
+        <v>44549</v>
       </c>
       <c r="C118" t="s">
         <v>23</v>
       </c>
       <c r="D118">
-        <v>175.1705357142879</v>
+        <v>172.564595238095</v>
       </c>
       <c r="E118">
-        <v>180.9860744791596</v>
+        <v>172.5371725861211</v>
       </c>
       <c r="F118">
-        <v>-5.815538764871661</v>
+        <v>0</v>
       </c>
       <c r="G118">
-        <v>-9.47685948239365</v>
+        <v>0</v>
       </c>
       <c r="H118">
-        <v>0.9678674794090785</v>
+        <v>1.00015893764551</v>
       </c>
       <c r="I118">
-        <v>1.576511399514425</v>
+        <v>1.579236706502634</v>
       </c>
       <c r="J118">
-        <v>1.591988371081941</v>
+        <v>1.579163589419889</v>
       </c>
       <c r="K118">
-        <v>375.7543095238119</v>
+        <v>375.0512321428673</v>
       </c>
       <c r="L118">
-        <v>592.3809523809524</v>
+        <v>592.2946726190477</v>
       </c>
       <c r="M118">
-        <v>40.6</v>
+        <v>27.9</v>
       </c>
     </row>
     <row r="119" spans="1:13">
       <c r="A119" s="1">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B119" s="3">
-        <v>44577</v>
+        <v>44556</v>
       </c>
       <c r="C119" t="s">
         <v>23</v>
       </c>
       <c r="D119">
-        <v>182.8107678571472</v>
+        <v>170.0147678571465</v>
       </c>
       <c r="E119">
-        <v>183.671769363045</v>
+        <v>171.4509159512136</v>
       </c>
       <c r="F119">
-        <v>-0.8610015058978036</v>
+        <v>0</v>
       </c>
       <c r="G119">
-        <v>-10.33786098829145</v>
+        <v>0</v>
       </c>
       <c r="H119">
-        <v>0.995312281746489</v>
+        <v>0.9916235612618378</v>
       </c>
       <c r="I119">
-        <v>1.600224805410661</v>
+        <v>1.560486156660549</v>
       </c>
       <c r="J119">
-        <v>1.602510406928294</v>
+        <v>1.564317780166184</v>
       </c>
       <c r="K119">
-        <v>376.7067440476191</v>
+        <v>374.8145119047591</v>
       </c>
       <c r="L119">
-        <v>602.8154761904761</v>
+        <v>584.8928571428571</v>
       </c>
       <c r="M119">
-        <v>46</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="120" spans="1:13">
       <c r="A120" s="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B120" s="3">
-        <v>44584</v>
+        <v>44563</v>
       </c>
       <c r="C120" t="s">
         <v>23</v>
       </c>
       <c r="D120">
-        <v>184.3406488095144</v>
+        <v>172.4510654761855</v>
       </c>
       <c r="E120">
-        <v>185.1431699821308</v>
+        <v>176.1123861937075</v>
       </c>
       <c r="F120">
-        <v>-0.8025211726163377</v>
+        <v>-3.661320717521988</v>
       </c>
       <c r="G120">
-        <v>-11.14038216090779</v>
+        <v>-3.661320717521988</v>
       </c>
       <c r="H120">
-        <v>0.9956654022252411</v>
+        <v>0.9792103167945559</v>
       </c>
       <c r="I120">
-        <v>1.597186272590634</v>
+        <v>1.573893975160251</v>
       </c>
       <c r="J120">
-        <v>1.599262409603678</v>
+        <v>1.583661666017127</v>
       </c>
       <c r="K120">
-        <v>386.54538095238</v>
+        <v>374.8399464285689</v>
       </c>
       <c r="L120">
-        <v>617.3849761904762</v>
+        <v>589.9583333333334</v>
       </c>
       <c r="M120">
-        <v>40.4</v>
+        <v>32.6</v>
       </c>
     </row>
     <row r="121" spans="1:13">
       <c r="A121" s="1">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B121" s="3">
-        <v>44591</v>
+        <v>44570</v>
       </c>
       <c r="C121" t="s">
         <v>23</v>
       </c>
       <c r="D121">
-        <v>181.4743392857213</v>
+        <v>175.1705357142879</v>
       </c>
       <c r="E121">
-        <v>183.6180578703975</v>
+        <v>180.9860744791596</v>
       </c>
       <c r="F121">
-        <v>-2.143718584676179</v>
+        <v>-5.815538764871661</v>
       </c>
       <c r="G121">
-        <v>-13.28410074558397</v>
+        <v>-9.47685948239365</v>
       </c>
       <c r="H121">
-        <v>0.988325121126217</v>
+        <v>0.9678674794090785</v>
       </c>
       <c r="I121">
-        <v>1.593329211930617</v>
+        <v>1.576511399514425</v>
       </c>
       <c r="J121">
-        <v>1.5989775253621</v>
+        <v>1.591988371081941</v>
       </c>
       <c r="K121">
-        <v>379.5325119047581</v>
+        <v>375.7543095238119</v>
       </c>
       <c r="L121">
-        <v>604.7202380952381</v>
+        <v>592.3809523809524</v>
       </c>
       <c r="M121">
-        <v>43</v>
+        <v>40.6</v>
       </c>
     </row>
     <row r="122" spans="1:13">
       <c r="A122" s="1">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B122" s="3">
-        <v>44598</v>
+        <v>44577</v>
       </c>
       <c r="C122" t="s">
         <v>23</v>
       </c>
       <c r="D122">
-        <v>186.8434761904757</v>
+        <v>182.8107678571472</v>
       </c>
       <c r="E122">
-        <v>184.8688709310774</v>
+        <v>183.671769363045</v>
       </c>
       <c r="F122">
-        <v>1.974605259398231</v>
+        <v>-0.8610015058978036</v>
       </c>
       <c r="G122">
-        <v>-11.30949548618574</v>
+        <v>-10.33786098829145</v>
       </c>
       <c r="H122">
-        <v>1.010681112777145</v>
+        <v>0.995312281746489</v>
       </c>
       <c r="I122">
-        <v>1.61358206786293</v>
+        <v>1.600224805410661</v>
       </c>
       <c r="J122">
-        <v>1.608401307699431</v>
+        <v>1.602510406928294</v>
       </c>
       <c r="K122">
-        <v>381.1419940476272</v>
+        <v>376.7067440476191</v>
       </c>
       <c r="L122">
-        <v>615.0038869047619</v>
+        <v>602.8154761904761</v>
       </c>
       <c r="M122">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="123" spans="1:13">
       <c r="A123" s="1">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B123" s="3">
-        <v>44605</v>
+        <v>44584</v>
       </c>
       <c r="C123" t="s">
         <v>23</v>
       </c>
       <c r="D123">
-        <v>197.7116547619059</v>
+        <v>184.3406488095144</v>
       </c>
       <c r="E123">
-        <v>185.8840415287217</v>
+        <v>185.1431699821308</v>
       </c>
       <c r="F123">
-        <v>11.82761323318425</v>
+        <v>-0.8025211726163377</v>
       </c>
       <c r="G123">
-        <v>0.518117746998513</v>
+        <v>-11.14038216090779</v>
       </c>
       <c r="H123">
-        <v>1.063628986845311</v>
+        <v>0.9956654022252411</v>
       </c>
       <c r="I123">
-        <v>1.639602237824401</v>
+        <v>1.597186272590634</v>
       </c>
       <c r="J123">
-        <v>1.60875669308516</v>
+        <v>1.599262409603678</v>
       </c>
       <c r="K123">
-        <v>383.4464047618953</v>
+        <v>386.54538095238</v>
       </c>
       <c r="L123">
-        <v>628.6995833333333</v>
+        <v>617.3849761904762</v>
       </c>
       <c r="M123">
-        <v>44.9</v>
+        <v>40.4</v>
       </c>
     </row>
     <row r="124" spans="1:13">
       <c r="A124" s="1">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B124" s="3">
-        <v>44612</v>
+        <v>44591</v>
       </c>
       <c r="C124" t="s">
         <v>23</v>
       </c>
       <c r="D124">
-        <v>197.7937559523797</v>
+        <v>181.4743392857213</v>
       </c>
       <c r="E124">
-        <v>187.2491318869175</v>
+        <v>183.6180578703975</v>
       </c>
       <c r="F124">
-        <v>10.54462406546222</v>
+        <v>-2.143718584676179</v>
       </c>
       <c r="G124">
-        <v>11.06274181246073</v>
+        <v>-13.28410074558397</v>
       </c>
       <c r="H124">
-        <v>1.05631334019658</v>
+        <v>0.988325121126217</v>
       </c>
       <c r="I124">
-        <v>1.615389789850532</v>
+        <v>1.593329211930617</v>
       </c>
       <c r="J124">
-        <v>1.588496278023952</v>
+        <v>1.5989775253621</v>
       </c>
       <c r="K124">
-        <v>392.0880297619095</v>
+        <v>379.5325119047581</v>
       </c>
       <c r="L124">
-        <v>633.375</v>
+        <v>604.7202380952381</v>
       </c>
       <c r="M124">
-        <v>39.9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="125" spans="1:13">
       <c r="A125" s="1">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B125" s="3">
-        <v>44619</v>
+        <v>44598</v>
       </c>
       <c r="C125" t="s">
         <v>23</v>
       </c>
       <c r="D125">
-        <v>194.8063809523758</v>
+        <v>186.8434761904757</v>
       </c>
       <c r="E125">
-        <v>186.0622762453148</v>
+        <v>184.8688709310774</v>
       </c>
       <c r="F125">
-        <v>8.744104707060984</v>
+        <v>1.974605259398231</v>
       </c>
       <c r="G125">
-        <v>19.80684651952171</v>
+        <v>-11.30949548618574</v>
       </c>
       <c r="H125">
-        <v>1.046995580638454</v>
+        <v>1.010681112777145</v>
       </c>
       <c r="I125">
-        <v>1.613001273864715</v>
+        <v>1.61358206786293</v>
       </c>
       <c r="J125">
-        <v>1.590289983548631</v>
+        <v>1.608401307699431</v>
       </c>
       <c r="K125">
-        <v>385.0113571428616</v>
+        <v>381.1419940476272</v>
       </c>
       <c r="L125">
-        <v>621.0238095238095</v>
+        <v>615.0038869047619</v>
       </c>
       <c r="M125">
-        <v>43.6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="126" spans="1:13">
       <c r="A126" s="1">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B126" s="3">
-        <v>44626</v>
+        <v>44605</v>
       </c>
       <c r="C126" t="s">
         <v>23</v>
       </c>
       <c r="D126">
-        <v>190.078869047619</v>
+        <v>197.7116547619059</v>
       </c>
       <c r="E126">
-        <v>181.811394568756</v>
+        <v>185.8840415287217</v>
       </c>
       <c r="F126">
-        <v>8.267474478863022</v>
+        <v>11.82761323318425</v>
       </c>
       <c r="G126">
-        <v>28.07432099838474</v>
+        <v>0.518117746998513</v>
       </c>
       <c r="H126">
-        <v>1.045472807127809</v>
+        <v>1.063628986845311</v>
       </c>
       <c r="I126">
-        <v>1.613921658484486</v>
+        <v>1.639602237824401</v>
       </c>
       <c r="J126">
-        <v>1.59242886934804</v>
+        <v>1.60875669308516</v>
       </c>
       <c r="K126">
-        <v>384.6627083333275</v>
+        <v>383.4464047618953</v>
       </c>
       <c r="L126">
-        <v>620.8154761904761</v>
+        <v>628.6995833333333</v>
       </c>
       <c r="M126">
-        <v>42.2</v>
+        <v>44.9</v>
       </c>
     </row>
     <row r="127" spans="1:13">
       <c r="A127" s="1">
+        <v>59</v>
+      </c>
+      <c r="B127" s="3">
+        <v>44612</v>
+      </c>
+      <c r="C127" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127">
+        <v>197.7937559523797</v>
+      </c>
+      <c r="E127">
+        <v>187.2491318869175</v>
+      </c>
+      <c r="F127">
+        <v>10.54462406546222</v>
+      </c>
+      <c r="G127">
+        <v>11.06274181246073</v>
+      </c>
+      <c r="H127">
+        <v>1.05631334019658</v>
+      </c>
+      <c r="I127">
+        <v>1.615389789850532</v>
+      </c>
+      <c r="J127">
+        <v>1.588496278023952</v>
+      </c>
+      <c r="K127">
+        <v>392.0880297619095</v>
+      </c>
+      <c r="L127">
+        <v>633.375</v>
+      </c>
+      <c r="M127">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
+      <c r="A128" s="1">
+        <v>60</v>
+      </c>
+      <c r="B128" s="3">
+        <v>44619</v>
+      </c>
+      <c r="C128" t="s">
+        <v>23</v>
+      </c>
+      <c r="D128">
+        <v>194.8063809523758</v>
+      </c>
+      <c r="E128">
+        <v>186.0622762453148</v>
+      </c>
+      <c r="F128">
+        <v>8.744104707060984</v>
+      </c>
+      <c r="G128">
+        <v>19.80684651952171</v>
+      </c>
+      <c r="H128">
+        <v>1.046995580638454</v>
+      </c>
+      <c r="I128">
+        <v>1.613001273864715</v>
+      </c>
+      <c r="J128">
+        <v>1.590289983548631</v>
+      </c>
+      <c r="K128">
+        <v>385.0113571428616</v>
+      </c>
+      <c r="L128">
+        <v>621.0238095238095</v>
+      </c>
+      <c r="M128">
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13">
+      <c r="A129" s="1">
+        <v>61</v>
+      </c>
+      <c r="B129" s="3">
+        <v>44626</v>
+      </c>
+      <c r="C129" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129">
+        <v>190.078869047619</v>
+      </c>
+      <c r="E129">
+        <v>185.2952572260893</v>
+      </c>
+      <c r="F129">
+        <v>4.783611821529718</v>
+      </c>
+      <c r="G129">
+        <v>24.59045834105143</v>
+      </c>
+      <c r="H129">
+        <v>1.025816158994793</v>
+      </c>
+      <c r="I129">
+        <v>1.613921658484486</v>
+      </c>
+      <c r="J129">
+        <v>1.601485797877525</v>
+      </c>
+      <c r="K129">
+        <v>384.6627083333275</v>
+      </c>
+      <c r="L129">
+        <v>620.8154761904761</v>
+      </c>
+      <c r="M129">
+        <v>42.2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13">
+      <c r="A130" s="1">
         <v>62</v>
       </c>
-      <c r="B127" s="3">
+      <c r="B130" s="3">
         <v>44633</v>
       </c>
-      <c r="C127" t="s">
-        <v>23</v>
-      </c>
-      <c r="D127">
-        <v>182.6049999999814</v>
-      </c>
-      <c r="E127">
-        <v>159.9790901560654</v>
-      </c>
-      <c r="F127">
-        <v>22.62590984391593</v>
-      </c>
-      <c r="G127">
-        <v>50.70023084230067</v>
-      </c>
-      <c r="H127">
-        <v>1.14143041957448</v>
-      </c>
-      <c r="I127">
-        <v>1.575699045392223</v>
-      </c>
-      <c r="J127">
-        <v>1.516721999003159</v>
-      </c>
-      <c r="K127">
-        <v>383.6392500000075</v>
-      </c>
-      <c r="L127">
-        <v>604.5</v>
+      <c r="C130" t="s">
+        <v>23</v>
+      </c>
+      <c r="D130">
+        <v>197.1086904762002</v>
+      </c>
+      <c r="E130">
+        <v>185.251300880667</v>
+      </c>
+      <c r="F130">
+        <v>11.85738959553322</v>
+      </c>
+      <c r="G130">
+        <v>36.44784793658465</v>
+      </c>
+      <c r="H130">
+        <v>1.064007051713884</v>
+      </c>
+      <c r="I130">
+        <v>1.625865329993205</v>
+      </c>
+      <c r="J130">
+        <v>1.595175665906781</v>
+      </c>
+      <c r="K130">
+        <v>386.3642678571466</v>
+      </c>
+      <c r="L130">
+        <v>628.1762678571429</v>
+      </c>
+      <c r="M130">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
+      <c r="A131" s="1">
+        <v>63</v>
+      </c>
+      <c r="B131" s="3">
+        <v>44640</v>
+      </c>
+      <c r="C131" t="s">
+        <v>23</v>
+      </c>
+      <c r="D131">
+        <v>193.7589999999895</v>
+      </c>
+      <c r="E131">
+        <v>177.3863615043983</v>
+      </c>
+      <c r="F131">
+        <v>16.37263849559127</v>
+      </c>
+      <c r="G131">
+        <v>52.82048643217593</v>
+      </c>
+      <c r="H131">
+        <v>1.092299308451542</v>
+      </c>
+      <c r="I131">
+        <v>1.610143771924244</v>
+      </c>
+      <c r="J131">
+        <v>1.567829084876882</v>
+      </c>
+      <c r="K131">
+        <v>386.9256666666618</v>
+      </c>
+      <c r="L131">
+        <v>623.0059523809524</v>
+      </c>
+      <c r="M131">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13">
+      <c r="A132" s="1">
+        <v>64</v>
+      </c>
+      <c r="B132" s="3">
+        <v>44647</v>
+      </c>
+      <c r="C132" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132">
+        <v>185.9311845238165</v>
+      </c>
+      <c r="E132">
+        <v>176.4547806342112</v>
+      </c>
+      <c r="F132">
+        <v>9.476403889605308</v>
+      </c>
+      <c r="G132">
+        <v>62.29689032178123</v>
+      </c>
+      <c r="H132">
+        <v>1.053704432691171</v>
+      </c>
+      <c r="I132">
+        <v>1.588890099230065</v>
+      </c>
+      <c r="J132">
+        <v>1.564450753840787</v>
+      </c>
+      <c r="K132">
+        <v>387.7519523809564</v>
+      </c>
+      <c r="L132">
+        <v>616.0952380952381</v>
+      </c>
+      <c r="M132">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
+      <c r="A133" s="1">
+        <v>65</v>
+      </c>
+      <c r="B133" s="3">
+        <v>44654</v>
+      </c>
+      <c r="C133" t="s">
+        <v>23</v>
+      </c>
+      <c r="D133">
+        <v>199.28085416666</v>
+      </c>
+      <c r="E133">
+        <v>162.1769312969526</v>
+      </c>
+      <c r="F133">
+        <v>37.10392286970742</v>
+      </c>
+      <c r="G133">
+        <v>99.40081319148865</v>
+      </c>
+      <c r="H133">
+        <v>1.228786687311086</v>
+      </c>
+      <c r="I133">
+        <v>1.630198047474724</v>
+      </c>
+      <c r="J133">
+        <v>1.53479309066739</v>
+      </c>
+      <c r="K133">
+        <v>388.9098020833238</v>
+      </c>
+      <c r="L133">
+        <v>634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>